<commit_message>
bug fix: tratamento coluna excel
</commit_message>
<xml_diff>
--- a/documents/excel_arquivos/excel_tratado.xlsx
+++ b/documents/excel_arquivos/excel_tratado.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E128"/>
+  <dimension ref="A1:E107"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,1082 +467,1082 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>CC-0001  - EC_CONTABILIDADE</t>
+          <t>CC-0002 - EC_FINANCEIRO</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>CAIXA ECONOMICA FEDERAL</t>
+          <t>DECIMO QUARTO TABELIONATO DE NOTAS</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>NF Nº 27102022</t>
+          <t>NF Nº 09012023</t>
         </is>
       </c>
       <c r="D2" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E2" t="n">
-        <v>476.55</v>
+        <v>18.9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>CC-0002  - EC_FINANCEIRO</t>
+          <t>CC-0002 - EC_FINANCEIRO</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>CAIXA ECONOMICA FEDERAL</t>
+          <t>FABIO FRANCISCO OLIVEIRA DA SILVA</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>NF Nº 27102022</t>
+          <t>NF Nº 09012023</t>
         </is>
       </c>
       <c r="D3" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E3" t="n">
-        <v>543.73</v>
+        <v>762</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>CC-0003  - EC_ADMINISTRAÇÃO</t>
+          <t>CC-0002 - EC_FINANCEIRO</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>CAIXA ECONOMICA FEDERAL</t>
+          <t>LM TRANSPORTES INTERESTADUAIS SERVICOS E COMERCIO S.A</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>NF Nº 27102022</t>
+          <t>NF Nº 00031437</t>
         </is>
       </c>
       <c r="D4" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E4" t="n">
-        <v>915.84</v>
+        <v>2439</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CC-0003  - EC_ADMINISTRAÇÃO</t>
+          <t>CC-0004 - EC_RECURSOS HUMANOS</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>LAERTE MENDES DE SOUZA</t>
+          <t>CONDOMINIO EDIFICIO ATHENAS</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>NF Nº 00042022</t>
+          <t>NF Nº 00012023-1</t>
         </is>
       </c>
       <c r="D5" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E5" t="n">
-        <v>1224</v>
+        <v>15417.08</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>CC-0003  - EC_ADMINISTRAÇÃO</t>
+          <t>CC-0004 - EC_RECURSOS HUMANOS</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>LAERTE MENDES DE SOUZA</t>
+          <t>CONSTRUTORA FONSECA &amp; MERCADANTE LTDA</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>NF Nº 00102022</t>
+          <t>NF Nº 05822023</t>
         </is>
       </c>
       <c r="D6" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E6" t="n">
-        <v>108.5</v>
+        <v>18515.59</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>CC-0003  - EC_ADMINISTRAÇÃO</t>
+          <t>CC-0004 - EC_RECURSOS HUMANOS</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>LAERTE MENDES DE SOUZA</t>
+          <t>CONSTRUTORA FONSECA &amp; MERCADANTE LTDA</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>NF Nº 00112022</t>
+          <t>NF Nº 05902023</t>
         </is>
       </c>
       <c r="D7" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E7" t="n">
-        <v>250</v>
+        <v>16166.52</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CC-0003  - EC_ADMINISTRAÇÃO</t>
+          <t>CC-0004 - EC_RECURSOS HUMANOS</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>LAERTE MENDES DE SOUZA</t>
+          <t>MARIO DILSON XAVIER SOARES</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>NF Nº 01202227</t>
+          <t>NF Nº 03012023</t>
         </is>
       </c>
       <c r="D8" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E8" t="n">
-        <v>622.15</v>
+        <v>720</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CC-0003  - EC_ADMINISTRAÇÃO</t>
+          <t>CC-0004 - EC_RECURSOS HUMANOS</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>LAERTE MENDES DE SOUZA</t>
+          <t>SINDICATO DA INDUSTRIA DA CONSTRUCAO CIVIL DE GRANDES ESTRUTURAS NO ESTADO DE SAO PAULO</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>NF Nº 02202227</t>
+          <t>NF Nº 01202300-1</t>
         </is>
       </c>
       <c r="D9" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E9" t="n">
-        <v>471.5</v>
+        <v>1764</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CC-0004  - EC_RECURSOS HUMANOS</t>
+          <t>CC-0005 - EC_JURÍDICO</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>CAIXA ECONOMICA FEDERAL</t>
+          <t>KINEA RENDA IMOBILIARIA FUNDO DE INVESTIMENTO IMOBILIARIO - FII</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>NF Nº 27102022</t>
+          <t>NF Nº 00092301</t>
         </is>
       </c>
       <c r="D10" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E10" t="n">
-        <v>1681.94</v>
+        <v>6213.76</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>CC-0004  - EC_RECURSOS HUMANOS</t>
+          <t>CC-0005 - EC_JURÍDICO</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>EVERTON MACHADO 32468201809</t>
+          <t>KONAI, ANDRADE ADVOGADOS ASSOCIADOS</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>NF Nº 00000132</t>
+          <t>NF Nº 09012023</t>
         </is>
       </c>
       <c r="D11" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E11" t="n">
-        <v>358.7</v>
+        <v>82.8</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CC-0004  - EC_RECURSOS HUMANOS</t>
+          <t>CC-0005 - EC_JURÍDICO</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>SALES EQUIPAMENTOS E PRODUTOS DE HIGIENE PROFISSIONAL LTDA</t>
+          <t>KONAI, ANDRADE ADVOGADOS ASSOCIADOS</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>NF Nº 04591167</t>
+          <t>NF Nº 20230901</t>
         </is>
       </c>
       <c r="D12" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E12" t="n">
-        <v>2000</v>
+        <v>16103</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>CC-0004  - EC_RECURSOS HUMANOS</t>
+          <t>CC-0005 - EC_JURÍDICO</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>SUL AMERICA COMPANHIA DE SEGURO SAUDE</t>
+          <t>TOKIO MARINE SEGURADORA S.A.</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>NF Nº 08423749-0</t>
+          <t>NF Nº 02591307</t>
         </is>
       </c>
       <c r="D13" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E13" t="n">
-        <v>38.04</v>
+        <v>761.75</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>CC-0005  - EC_JURÍDICO</t>
+          <t>CC-0006 - EC_TI</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>CAIXA ECONOMICA FEDERAL</t>
+          <t>GR COMERCIO E MANUTENCAO DE COMPUTADORES LTDA - ME</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>NF Nº 27102022</t>
+          <t>NF Nº 00004158</t>
         </is>
       </c>
       <c r="D14" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E14" t="n">
-        <v>942.77</v>
+        <v>3366.31</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>CC-0005  - EC_JURÍDICO</t>
+          <t>CC-0006 - EC_TI</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>CONDOMINIO EDIFICIO ATHENAS</t>
+          <t>TELEFONICA CLOUD E TECNOLOGIA DO BRASIL S.A.</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>NF Nº 00660090</t>
+          <t>NF Nº 700405037</t>
         </is>
       </c>
       <c r="D15" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E15" t="n">
-        <v>15009.22</v>
+        <v>3082.1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>CC-0005  - EC_JURÍDICO</t>
+          <t>CC-0007 - EC_SUPRIMENTOS</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>KINEA RENDA IMOBILIARIA FUNDO DE INVESTIMENTO IMOBILIARIO - FII</t>
+          <t>WADSON MALAQUIAS DA SILVA</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>NF Nº 00003505</t>
+          <t>NF Nº 09012023</t>
         </is>
       </c>
       <c r="D16" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E16" t="n">
-        <v>6213.76</v>
+        <v>284.93</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>CC-0005  - EC_JURÍDICO</t>
+          <t>CC-0009 - EC_COMERCIAL</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>KONAI, ANDRADE ADVOGADOS ASSOCIADOS</t>
+          <t>Cêra Sociedade de Advogados</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>NF Nº 00000616</t>
+          <t>NF Nº 00003676</t>
         </is>
       </c>
       <c r="D17" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E17" t="n">
-        <v>15834</v>
+        <v>3800.92</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>CC-0005  - EC_JURÍDICO</t>
+          <t>CC-0010 - EC_ENGENHARIA</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>LIBERTY SEGUROS S/A</t>
+          <t>KALUNGA SA</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>NF Nº 00039000</t>
+          <t>NF Nº 00201222</t>
         </is>
       </c>
       <c r="D18" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E18" t="n">
-        <v>1241.63</v>
+        <v>72.63</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>CC-0005  - EC_JURÍDICO</t>
+          <t>CC-0240 - FARIA LIMA PLAZA - FLP</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>SUL AMERICA COMPANHIA DE SEGURO SAUDE</t>
+          <t>AUGUSTO DE CARVALHO MARTINS</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>NF Nº 08423749-0</t>
+          <t>NF Nº 00012023</t>
         </is>
       </c>
       <c r="D19" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E19" t="n">
-        <v>38.04</v>
+        <v>83.06999999999999</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>CC-0005  - EC_JURÍDICO</t>
+          <t>CC-0240 - FARIA LIMA PLAZA - FLP</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>TOKIO MARINE SEGURADORA S.A.</t>
+          <t>AUGUSTO DE CARVALHO MARTINS</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>NF Nº 02591307</t>
+          <t>NF Nº 00022023</t>
         </is>
       </c>
       <c r="D20" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E20" t="n">
-        <v>126.96</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>CC-0006  - EC_TI</t>
+          <t>CC-0240 - FARIA LIMA PLAZA - FLP</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>CAIXA ECONOMICA FEDERAL</t>
+          <t>CARLOS PRESTES VAZ FIGUEIRA TRANSPORTES - ME</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>NF Nº 27102022</t>
+          <t>NF Nº 00027527</t>
         </is>
       </c>
       <c r="D21" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E21" t="n">
-        <v>891.78</v>
+        <v>560</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>CC-0006  - EC_TI</t>
+          <t>CC-0240 - FARIA LIMA PLAZA - FLP</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>MAV TECNOLOGIA LTDA</t>
+          <t>D.A. LOCACAO DE MAQUINAS E EQUIPAMENTOS LTDA</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>NF Nº 20223758</t>
+          <t>NF Nº 00005870</t>
         </is>
       </c>
       <c r="D22" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E22" t="n">
-        <v>1982.31</v>
+        <v>2400</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>CC-0006  - EC_TI</t>
+          <t>CC-0240 - FARIA LIMA PLAZA - FLP</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>SUL AMERICA COMPANHIA DE SEGURO SAUDE</t>
+          <t>D.A. LOCACAO DE MAQUINAS E EQUIPAMENTOS LTDA</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>NF Nº 08423749-0</t>
+          <t>NF Nº 00005951</t>
         </is>
       </c>
       <c r="D23" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E23" t="n">
-        <v>55.16</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>CC-0007  - EC_SUPRIMENTOS</t>
+          <t>CC-0246 - PASSEIO PAULISTA</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>BRASLIMPO COMERCIAL LTDA</t>
+          <t xml:space="preserve">ALINE DE SOUZA SANTOS </t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>NF Nº 00845625</t>
+          <t>NF Nº 00382022</t>
         </is>
       </c>
       <c r="D24" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E24" t="n">
-        <v>435.18</v>
+        <v>2399.35</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>CC-0007  - EC_SUPRIMENTOS</t>
+          <t>CC-0246 - PASSEIO PAULISTA</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>CAIXA ECONOMICA FEDERAL</t>
+          <t xml:space="preserve">GIOVANNI CREMASCO DONATO </t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>NF Nº 27102022</t>
+          <t>NF Nº 00332022</t>
         </is>
       </c>
       <c r="D25" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E25" t="n">
-        <v>4837.22</v>
+        <v>3002</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>CC-0007  - EC_SUPRIMENTOS</t>
+          <t>CC-0246 - PASSEIO PAULISTA</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>DOCUSIGN BRASIL SOLUCOES EM TECNOLOGIA LTDA.</t>
+          <t>Marcelo Aratan y de Melo Oliveira</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>NF Nº 00527263</t>
+          <t>NF Nº 00000001</t>
         </is>
       </c>
       <c r="D26" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E26" t="n">
-        <v>5189.17</v>
+        <v>8500</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>CC-0007  - EC_SUPRIMENTOS</t>
+          <t>CC-0246 - PASSEIO PAULISTA</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>DOCUSIGN BRASIL SOLUCOES EM TECNOLOGIA LTDA.</t>
+          <t>PAULO DE TARSO GOMES PEREIRA</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>NF Nº 00527264</t>
+          <t>NF Nº 00102022</t>
         </is>
       </c>
       <c r="D27" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E27" t="n">
-        <v>494.79</v>
+        <v>150</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>CC-0007  - EC_SUPRIMENTOS</t>
+          <t>CC-0246 - PASSEIO PAULISTA</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>SUL AMERICA COMPANHIA DE SEGURO SAUDE</t>
+          <t>PREFEITURA DE SÃO PAULO &lt;CONSTRUTORA FONSECA &amp; MERCADANTE LTDA&gt;</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>NF Nº 08423749-0</t>
+          <t>NF Nº 00002441</t>
         </is>
       </c>
       <c r="D28" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E28" t="n">
-        <v>76.08</v>
+        <v>20492.95</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>CC-0008  - EC_ORÇAMENTOS</t>
+          <t>CC-0246 - PASSEIO PAULISTA</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>CAIXA ECONOMICA FEDERAL</t>
+          <t>THAIS CRISTINA SILVA DO NASCIMENTO</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>NF Nº 27102022</t>
+          <t>NF Nº 00072022</t>
         </is>
       </c>
       <c r="D29" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E29" t="n">
-        <v>1803.56</v>
+        <v>150</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>CC-0008  - EC_ORÇAMENTOS</t>
+          <t>CC-0250 - HOSPITAL SÃO LUIZ CAMPINAS</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>SUL AMERICA COMPANHIA DE SEGURO SAUDE</t>
+          <t>ACAZ SERVICOS ESPECIALIZADOS TERCEIRIZADOS LTDA</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>NF Nº 08423749-0</t>
+          <t>NF Nº 00000639</t>
         </is>
       </c>
       <c r="D30" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E30" t="n">
-        <v>38.04</v>
+        <v>20128.18</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>CC-0010  - EC_ENGENHARIA</t>
+          <t>CC-0250 - HOSPITAL SÃO LUIZ CAMPINAS</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>CAIXA ECONOMICA FEDERAL</t>
+          <t>BREHNZ INSTALACAO E MANUTENCAO EIRELI</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>NF Nº 27102022</t>
+          <t>NF Nº 00000104-E</t>
         </is>
       </c>
       <c r="D31" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E31" t="n">
-        <v>1839.86</v>
+        <v>10555.78</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>CC-0011  - EC_DIRETORIA</t>
+          <t>CC-0250 - HOSPITAL SÃO LUIZ CAMPINAS</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>CAIXA ECONOMICA FEDERAL</t>
+          <t>COMPANHIA PAULISTA DE FORCA E LUZ</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>NF Nº 27102022</t>
+          <t>NF Nº 276110170-C</t>
         </is>
       </c>
       <c r="D32" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E32" t="n">
-        <v>635.42</v>
+        <v>142.23</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>CC-0011  - EC_DIRETORIA</t>
+          <t>CC-0250 - HOSPITAL SÃO LUIZ CAMPINAS</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>SECRETARIA DA FAZENDA DO ESTADO DE SÃO PAULO</t>
+          <t>COMPANHIA PAULISTA DE FORCA E LUZ</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>NF Nº 09112022</t>
+          <t>NF Nº 278194659-C</t>
         </is>
       </c>
       <c r="D33" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E33" t="n">
-        <v>426.44</v>
+        <v>38633.08</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>CC-0011  - EC_DIRETORIA</t>
+          <t>CC-0250 - HOSPITAL SÃO LUIZ CAMPINAS</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>SUL AMERICA COMPANHIA DE SEGURO SAUDE</t>
+          <t>COMPANHIA PAULISTA DE FORCA E LUZ</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>NF Nº 08423749-0</t>
+          <t>NF Nº 281133442-C</t>
         </is>
       </c>
       <c r="D34" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E34" t="n">
-        <v>19.02</v>
+        <v>158.38</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>CC-0013  - EC_SERVIÇOS GERAIS</t>
+          <t>CC-0250 - HOSPITAL SÃO LUIZ CAMPINAS</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>CAIXA ECONOMICA FEDERAL</t>
+          <t>EDSON YAMAZAKI</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>NF Nº 27102022</t>
+          <t>NF Nº 00232022</t>
         </is>
       </c>
       <c r="D35" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E35" t="n">
-        <v>605.15</v>
+        <v>368</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>CC-0013  - EC_SERVIÇOS GERAIS</t>
+          <t>CC-0250 - HOSPITAL SÃO LUIZ CAMPINAS</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>CAIXA ECONOMICA FEDERAL</t>
+          <t>EDSON YAMAZAKI</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>NF Nº 271020222</t>
+          <t>NF Nº 00242022</t>
         </is>
       </c>
       <c r="D36" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E36" t="n">
-        <v>27.26</v>
+        <v>200</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>CC-0013  - EC_SERVIÇOS GERAIS</t>
+          <t>CC-0250 - HOSPITAL SÃO LUIZ CAMPINAS</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>SUL AMERICA COMPANHIA DE SEGURO SAUDE</t>
+          <t>EDUARDO GOMES DA SILVA</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>NF Nº 08423749-0</t>
+          <t>NF Nº 00001822</t>
         </is>
       </c>
       <c r="D37" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E37" t="n">
-        <v>294.82</v>
+        <v>42.2</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>CC-0240 - FARIA LIMA PLAZA - FLP</t>
+          <t>CC-0250 - HOSPITAL SÃO LUIZ CAMPINAS</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>ENGEILHA AMBIENTAL TRANSPORTES, LOCACOES E TERRAPLANAGEM EIRELI</t>
+          <t>EDUARDO GOMES DA SILVA</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>NF Nº 00004575</t>
+          <t>NF Nº 00001922</t>
         </is>
       </c>
       <c r="D38" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E38" t="n">
-        <v>589</v>
+        <v>255.3</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>CC-0246 - PASSEIO PAULISTA</t>
+          <t>CC-0250 - HOSPITAL SÃO LUIZ CAMPINAS</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>ADRIANO DE GOUVEIA E FREITAS</t>
+          <t>EDUARDO GOMES DA SILVA</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>NF Nº 00092022</t>
+          <t>NF Nº 00192022</t>
         </is>
       </c>
       <c r="D39" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E39" t="n">
-        <v>165</v>
+        <v>180</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>CC-0246 - PASSEIO PAULISTA</t>
+          <t>CC-0250 - HOSPITAL SÃO LUIZ CAMPINAS</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>CAIXA ECONOMICA FEDERAL</t>
+          <t>EDUARDO GOMES DA SILVA</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>NF Nº 27102022</t>
+          <t>NF Nº 00222022</t>
         </is>
       </c>
       <c r="D40" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E40" t="n">
-        <v>19192.12</v>
+        <v>255.3</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>CC-0246 - PASSEIO PAULISTA</t>
+          <t>CC-0250 - HOSPITAL SÃO LUIZ CAMPINAS</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>EVERTON MACHADO 32468201809</t>
+          <t>FLAVIO COELHO LOPES</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>NF Nº 00000132</t>
+          <t>NF Nº 00001022</t>
         </is>
       </c>
       <c r="D41" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E41" t="n">
-        <v>1076.09</v>
+        <v>489.91</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>CC-0246 - PASSEIO PAULISTA</t>
+          <t>CC-0250 - HOSPITAL SÃO LUIZ CAMPINAS</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>FNEC - SERVICOS TECNICOS DE INSPECOES E TESTES LTDA</t>
+          <t>JA TOPOGRAFIA E LOCACAO LTDA</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>NF Nº 00001217</t>
+          <t>NF Nº 00000541</t>
         </is>
       </c>
       <c r="D42" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E42" t="n">
-        <v>6450</v>
+        <v>4350</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>CC-0246 - PASSEIO PAULISTA</t>
+          <t>CC-0250 - HOSPITAL SÃO LUIZ CAMPINAS</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>SUL AMERICA COMPANHIA DE SEGURO SAUDE</t>
+          <t>JOSIVAL BERTOLDO DA SILVA</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>NF Nº 08423749-0</t>
+          <t>NF Nº 00002222</t>
         </is>
       </c>
       <c r="D43" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E43" t="n">
-        <v>1029.98</v>
+        <v>180</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>CC-0246 - PASSEIO PAULISTA</t>
+          <t>CC-0250 - HOSPITAL SÃO LUIZ CAMPINAS</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>TELEFONICA BRASIL S.A.</t>
+          <t>JOSIVAL BERTOLDO DA SILVA</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>NF Nº 00920222</t>
+          <t>NF Nº 00222022</t>
         </is>
       </c>
       <c r="D44" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E44" t="n">
-        <v>119.59</v>
+        <v>602.6</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>CC-0246 - PASSEIO PAULISTA</t>
+          <t>CC-0250 - HOSPITAL SÃO LUIZ CAMPINAS</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>TELEFONICA BRASIL S.A.</t>
+          <t>JOSIVAL BERTOLDO DA SILVA</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>NF Nº 09202222</t>
+          <t>NF Nº 00232022</t>
         </is>
       </c>
       <c r="D45" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E45" t="n">
-        <v>3260.54</v>
+        <v>106.9</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>CC-0246 - PASSEIO PAULISTA</t>
+          <t>CC-0250 - HOSPITAL SÃO LUIZ CAMPINAS</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>TOKIO MARINE SEGURADORA S.A.</t>
+          <t>LUCAS GONZALEZ DA SILVA</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>NF Nº 02591307</t>
+          <t>NF Nº 00002122</t>
         </is>
       </c>
       <c r="D46" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E46" t="n">
-        <v>126.96</v>
+        <v>118.74</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>CC-0246 - PASSEIO PAULISTA</t>
+          <t>CC-0250 - HOSPITAL SÃO LUIZ CAMPINAS</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Thomas Silva</t>
+          <t>LUCAS GONZALEZ DA SILVA</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>NF Nº 28102022</t>
+          <t>NF Nº 00222022</t>
         </is>
       </c>
       <c r="D47" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E47" t="n">
-        <v>220</v>
+        <v>180</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>CC-0246 - PASSEIO PAULISTA</t>
+          <t>CC-0250 - HOSPITAL SÃO LUIZ CAMPINAS</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Thomas Silva</t>
+          <t>MARCOS ANTONIO ALBINO DE SOUZA</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>NF Nº 281020222</t>
+          <t>NF Nº 00252022</t>
         </is>
       </c>
       <c r="D48" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E48" t="n">
-        <v>23</v>
+        <v>725.65</v>
       </c>
     </row>
     <row r="49">
@@ -1553,19 +1553,19 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>ALVES PISOS INDUSTRIAIS EIRELI</t>
+          <t>MARIA CELINA DA COSTA BERNARDINO</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>NF Nº 00000194</t>
+          <t>NF Nº 00015990-0</t>
         </is>
       </c>
       <c r="D49" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E49" t="n">
-        <v>26840.88</v>
+        <v>5508</v>
       </c>
     </row>
     <row r="50">
@@ -1576,19 +1576,19 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>ARCA DAS FERRAMENTAS EIRELI –ME</t>
+          <t>MUNICIPIO DE CAMPINAS &lt;ACAZ SERVICOS ESPECIALIZADOS TERCEIRIZADOS LTDA&gt;</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>NF Nº 00005688-1</t>
+          <t>NF Nº 00000639</t>
         </is>
       </c>
       <c r="D50" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E50" t="n">
-        <v>2924.5</v>
+        <v>1198.1</v>
       </c>
     </row>
     <row r="51">
@@ -1599,19 +1599,19 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>CAIXA ECONOMICA FEDERAL</t>
+          <t>MUNICIPIO DE CAMPINAS &lt;ALESSANDRO JOSE AZEVEDO&gt;</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>NF Nº 27102022</t>
+          <t>NF Nº 00002690</t>
         </is>
       </c>
       <c r="D51" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E51" t="n">
-        <v>22124.2</v>
+        <v>151.55</v>
       </c>
     </row>
     <row r="52">
@@ -1622,19 +1622,19 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>COMPANHIA DE GAS DE SAO PAULO COMGAS</t>
+          <t>MUNICIPIO DE CAMPINAS &lt;ALESSANDRO JOSE AZEVEDO&gt;</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>NF Nº 74987610</t>
+          <t>NF Nº 00002691</t>
         </is>
       </c>
       <c r="D52" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E52" t="n">
-        <v>49.71</v>
+        <v>151.55</v>
       </c>
     </row>
     <row r="53">
@@ -1645,19 +1645,19 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>COMPANHIA PAULISTA DE FORCA E LUZ</t>
+          <t>MUNICIPIO DE CAMPINAS &lt;ALVES PISOS INDUSTRIAIS EIRELI&gt;</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>NF Nº 269785689-C</t>
+          <t>NF Nº 00000203</t>
         </is>
       </c>
       <c r="D53" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E53" t="n">
-        <v>133.77</v>
+        <v>1595.94</v>
       </c>
     </row>
     <row r="54">
@@ -1668,19 +1668,19 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>COMPANHIA PAULISTA DE FORCA E LUZ</t>
+          <t>MUNICIPIO DE CAMPINAS &lt;CONSTRUDAGER CONSTRUCOES LTDA&gt;</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>NF Nº 271207948</t>
+          <t>NF Nº 00000069</t>
         </is>
       </c>
       <c r="D54" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E54" t="n">
-        <v>157.9</v>
+        <v>5536.36</v>
       </c>
     </row>
     <row r="55">
@@ -1691,19 +1691,19 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>DARI MAXIMO ME</t>
+          <t>MUNICIPIO DE CAMPINAS &lt;EMPREITEIRA DE MAO DE OBRA MEGA ESTRUTURAS LTDA&gt;</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>NF Nº 00007939</t>
+          <t>NF Nº 00000086</t>
         </is>
       </c>
       <c r="D55" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E55" t="n">
-        <v>390.0400000000001</v>
+        <v>9127.219999999999</v>
       </c>
     </row>
     <row r="56">
@@ -1714,19 +1714,19 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>DARI MAXIMO ME</t>
+          <t>MUNICIPIO DE CAMPINAS &lt;ISAR ENGENHARIA E MONTAGENS LTDA&gt;</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>NF Nº 00007940</t>
+          <t>NF Nº 00004764</t>
         </is>
       </c>
       <c r="D56" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E56" t="n">
-        <v>1430</v>
+        <v>579.61</v>
       </c>
     </row>
     <row r="57">
@@ -1737,19 +1737,19 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>DEPOSITO DE MADEIRA SAO LUIZ LTDA</t>
+          <t>MUNICIPIO DE CAMPINAS &lt;L. C. F. SILVA SERVICOS E CONSTRUCOES&gt;</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>NF Nº 00626464-2</t>
+          <t>NF Nº 00000477</t>
         </is>
       </c>
       <c r="D57" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E57" t="n">
-        <v>175</v>
+        <v>2696.66</v>
       </c>
     </row>
     <row r="58">
@@ -1760,19 +1760,19 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>DRAGOES ESQUADRIAS METALICAS LTDA - ME</t>
+          <t>MUNICIPIO DE CAMPINAS &lt;LUCAS NOGUEIRA MARCAL VENTURA DO ROSARIO E SILVA&gt;</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>NF Nº 00000327</t>
+          <t>NF Nº 00001011</t>
         </is>
       </c>
       <c r="D58" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E58" t="n">
-        <v>17528.96</v>
+        <v>1403.27</v>
       </c>
     </row>
     <row r="59">
@@ -1783,19 +1783,19 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>ELIANE S/A - REVESTIMENTOS CERAMICOS</t>
+          <t>MUNICIPIO DE CAMPINAS &lt;SERVTEC SERVICOS EM OBRAS DE ENGENHARIA E COMERCIO DE MATERIAIS PARA CONSTRUCAO CIVIL EIRELI&gt;</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>NF Nº 00399013-1</t>
+          <t>NF Nº 00000683</t>
         </is>
       </c>
       <c r="D59" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E59" t="n">
-        <v>6209.059999999999</v>
+        <v>1858.99</v>
       </c>
     </row>
     <row r="60">
@@ -1806,19 +1806,19 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>EMPREITEIRA DE MAO DE OBRA MEGA ESTRUTURAS LTDA</t>
+          <t>MUNICIPIO DE CAMPINAS &lt;SERVTEC SERVICOS EM OBRAS DE ENGENHARIA E COMERCIO DE MATERIAIS PARA CONSTRUCAO CIVIL EIRELI&gt;</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>NF Nº 00000074</t>
+          <t>NF Nº 00000695</t>
         </is>
       </c>
       <c r="D60" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E60" t="n">
-        <v>122307.74</v>
+        <v>3884.4</v>
       </c>
     </row>
     <row r="61">
@@ -1829,19 +1829,19 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>EMPREITEIRA DE MAO DE OBRA MEGA ESTRUTURAS LTDA</t>
+          <t>MUNICIPIO DE CAMPINAS &lt;SMR TERRAPLENAGEM LTDA - EPP&gt;</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>NF Nº 00112022</t>
+          <t>NF Nº 00000357</t>
         </is>
       </c>
       <c r="D61" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E61" t="n">
-        <v>87176.32999999999</v>
+        <v>377.16</v>
       </c>
     </row>
     <row r="62">
@@ -1852,19 +1852,19 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>EVERTON MACHADO 32468201809</t>
+          <t>MUNICIPIO DE CAMPINAS &lt;SUPER OBRAS LTDA&gt;</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>NF Nº 00000132</t>
+          <t>NF Nº 00000009</t>
         </is>
       </c>
       <c r="D62" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E62" t="n">
-        <v>130.43</v>
+        <v>888.42</v>
       </c>
     </row>
     <row r="63">
@@ -1875,19 +1875,19 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>HENRIQUE DE SOUSA COELHO ZULLO</t>
+          <t>MUNICIPIO DE CAMPINAS &lt;SUPER OBRAS LTDA&gt;</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>NF Nº 00002856-001</t>
+          <t>NF Nº 00000010</t>
         </is>
       </c>
       <c r="D63" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E63" t="n">
-        <v>660</v>
+        <v>2651.03</v>
       </c>
     </row>
     <row r="64">
@@ -1898,19 +1898,19 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>LUCAS GONZALEZ DA SILVA</t>
+          <t>NATANAEL DOMINGOS VIEIRA</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>NF Nº 00162022</t>
+          <t>NF Nº 00032022</t>
         </is>
       </c>
       <c r="D64" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E64" t="n">
-        <v>180</v>
+        <v>412.1</v>
       </c>
     </row>
     <row r="65">
@@ -1921,19 +1921,19 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>M.V. AMBULANCIAS E REMOCOES LTDA</t>
+          <t>PERTECNICA HSMA CONSULTORIA E PROJETOS LIMITADA</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>NF Nº 00000632</t>
+          <t>NF Nº 00000237</t>
         </is>
       </c>
       <c r="D65" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E65" t="n">
-        <v>1200</v>
+        <v>2719.77</v>
       </c>
     </row>
     <row r="66">
@@ -1944,19 +1944,19 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>MILLS ESTRUTURAS E SERVICOS DE ENGENHARIA S/A</t>
+          <t>PIZZIMENTI FERRAGENS E FERRAMENTAS LTDA</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>NF Nº 910045295</t>
+          <t>NF Nº 00470366-1</t>
         </is>
       </c>
       <c r="D66" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E66" t="n">
-        <v>3593.14</v>
+        <v>22810.49</v>
       </c>
     </row>
     <row r="67">
@@ -1967,19 +1967,19 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>NH ESTRUTURAS TECNICAS LTDA</t>
+          <t>Paula Lemos de Almeida</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>NF Nº 00000225-1</t>
+          <t>NF Nº 00001222</t>
         </is>
       </c>
       <c r="D67" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E67" t="n">
-        <v>72019.60000000001</v>
+        <v>180</v>
       </c>
     </row>
     <row r="68">
@@ -1990,19 +1990,19 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Nayara Mendes Gonçalves</t>
+          <t>RODRIGO NAPOLITANO SCHALCH LOPES</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>NF Nº 00024738</t>
+          <t>NF Nº 00002022</t>
         </is>
       </c>
       <c r="D68" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E68" t="n">
-        <v>2446.67</v>
+        <v>1230.6</v>
       </c>
     </row>
     <row r="69">
@@ -2013,19 +2013,19 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Paula Lemos de Almeida</t>
+          <t>RODRIGO NAPOLITANO SCHALCH LOPES</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>NF Nº 31102022</t>
+          <t>NF Nº 00212022</t>
         </is>
       </c>
       <c r="D69" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E69" t="n">
-        <v>2500</v>
+        <v>296.49</v>
       </c>
     </row>
     <row r="70">
@@ -2036,19 +2036,19 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>ROSANA MARTINS DE FREITAS</t>
+          <t>Supermix Concreto S/A</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>NF Nº 00092022</t>
+          <t>NF Nº 00026329</t>
         </is>
       </c>
       <c r="D70" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E70" t="n">
-        <v>752.02</v>
+        <v>16356.62</v>
       </c>
     </row>
     <row r="71">
@@ -2059,19 +2059,19 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>SINDICATO DOS TRABALHADORES NAS INDUSTRIAS DA CONST CIVIL E DO MOBILIARIO DE CAMPINAS</t>
+          <t>TWO WAY EQUIPAMENTOS DE RADIOCOMUNICACAO LTDA</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>NF Nº 281020222</t>
+          <t>NF Nº 00001246</t>
         </is>
       </c>
       <c r="D71" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E71" t="n">
-        <v>488.49</v>
+        <v>825</v>
       </c>
     </row>
     <row r="72">
@@ -2082,19 +2082,19 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>SOCIEDADE DE ABASTECIMENTO DE AGUA E SANEAMENTO SA</t>
+          <t>VOTORANTIM CIMENTOS S.A.</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>NF Nº 04355391</t>
+          <t>NF Nº 00465351-6</t>
         </is>
       </c>
       <c r="D72" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E72" t="n">
-        <v>455.35</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="73">
@@ -2105,19 +2105,19 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>SOCIEDADE DE ABASTECIMENTO DE AGUA E SANEAMENTO SA</t>
+          <t>VOTORANTIM CIMENTOS S.A.</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>NF Nº 04523613</t>
+          <t>NF Nº 00465863-6</t>
         </is>
       </c>
       <c r="D73" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E73" t="n">
-        <v>163.67</v>
+        <v>6207.6</v>
       </c>
     </row>
     <row r="74">
@@ -2128,410 +2128,410 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>SOEDRAL SOCIEDADE ELETRICA HIDRAULICA LTDA</t>
+          <t>WILLIAN SILVESTRE DOS SANTOS</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>NF Nº 00249938</t>
+          <t>NF Nº 00092022</t>
         </is>
       </c>
       <c r="D74" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E74" t="n">
-        <v>7972.86</v>
+        <v>380.88</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>CC-0250 - HOSPITAL SÃO LUIZ CAMPINAS</t>
+          <t>CC-0251 - EDIFICIO VIVA!</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>SQUARE TRAVEL AGENCIA DE VIAGENS E TURISMO - EIRELI</t>
+          <t>PREFEITURA DE SÃO PAULO &lt;CONSTRUTORA FONSECA &amp; MERCADANTE LTDA&gt;</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>NF Nº 00004193</t>
+          <t>NF Nº 00002433</t>
         </is>
       </c>
       <c r="D75" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E75" t="n">
-        <v>894</v>
+        <v>501.4</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>CC-0250 - HOSPITAL SÃO LUIZ CAMPINAS</t>
+          <t>CC-0251 - EDIFICIO VIVA!</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>SUL AMERICA COMPANHIA DE SEGURO SAUDE</t>
+          <t>PREFEITURA DE SÃO PAULO &lt;CONSTRUTORA FONSECA &amp; MERCADANTE LTDA&gt;</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>NF Nº 08423749-0</t>
+          <t>NF Nº 00002434</t>
         </is>
       </c>
       <c r="D76" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E76" t="n">
-        <v>770.3200000000001</v>
+        <v>17635.09</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>CC-0250 - HOSPITAL SÃO LUIZ CAMPINAS</t>
+          <t>CC-0251 - EDIFICIO VIVA!</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>SUPER OBRAS LTDA</t>
+          <t>PREFEITURA DE SÃO PAULO &lt;CONSTRUTORA FONSECA &amp; MERCADANTE LTDA&gt;</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>NF Nº 00000006</t>
+          <t>NF Nº 00002435</t>
         </is>
       </c>
       <c r="D77" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E77" t="n">
-        <v>65478.75000000001</v>
+        <v>1836.25</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>CC-0250 - HOSPITAL SÃO LUIZ CAMPINAS</t>
+          <t>CC-0251 - EDIFICIO VIVA!</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>SUPER OBRAS LTDA</t>
+          <t>PREFEITURA DE SÃO PAULO &lt;CONSTRUTORA FONSECA &amp; MERCADANTE LTDA&gt;</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>NF Nº 00000007</t>
+          <t>NF Nº 00002439</t>
         </is>
       </c>
       <c r="D78" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E78" t="n">
-        <v>58343.52</v>
+        <v>10801.15</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>CC-0250 - HOSPITAL SÃO LUIZ CAMPINAS</t>
+          <t>CC-0251 - EDIFICIO VIVA!</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Supermix Concreto S/A</t>
+          <t>PREFEITURA DE SÃO PAULO &lt;CONSTRUTORA FONSECA &amp; MERCADANTE LTDA&gt;</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>NF Nº 00025899</t>
+          <t>NF Nº 00002443</t>
         </is>
       </c>
       <c r="D79" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E79" t="n">
-        <v>18127.58</v>
+        <v>13960</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>CC-0250 - HOSPITAL SÃO LUIZ CAMPINAS</t>
+          <t>CC-0251 - EDIFICIO VIVA!</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>TOKIO MARINE SEGURADORA S.A.</t>
+          <t>PREFEITURA DE SÃO PAULO &lt;CONSTRUTORA FONSECA &amp; MERCADANTE LTDA&gt;</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>NF Nº 02591307</t>
+          <t>NF Nº 00002446</t>
         </is>
       </c>
       <c r="D80" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E80" t="n">
-        <v>126.96</v>
+        <v>17635.09</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>CC-0250 - HOSPITAL SÃO LUIZ CAMPINAS</t>
+          <t>CC-0251 - EDIFICIO VIVA!</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>TRANSPORTES GEMEAS DO IGUACU LTDA</t>
+          <t>PREFEITURA DE SÃO PAULO &lt;CONSTRUTORA FONSECA &amp; MERCADANTE LTDA&gt;</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>NF Nº 00022630-1</t>
+          <t>NF Nº 00002447</t>
         </is>
       </c>
       <c r="D81" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E81" t="n">
-        <v>2430.01</v>
+        <v>1836.25</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>CC-0250 - HOSPITAL SÃO LUIZ CAMPINAS</t>
+          <t>CC-0251 - EDIFICIO VIVA!</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Thomas Silva</t>
+          <t>PREFEITURA DE SÃO PAULO &lt;CONSTRUTORA FONSECA &amp; MERCADANTE LTDA&gt;</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>NF Nº 281020222</t>
+          <t>NF Nº 00002449</t>
         </is>
       </c>
       <c r="D82" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E82" t="n">
-        <v>155.25</v>
+        <v>501.4</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>CC-0250 - HOSPITAL SÃO LUIZ CAMPINAS</t>
+          <t>CC-0251 - EDIFICIO VIVA!</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>VOTORANTIM CIMENTOS S.A.</t>
+          <t>PREFEITURA DE SÃO PAULO &lt;MEP SOLUTIONS LTDA&gt;</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>NF Nº 00456992-6</t>
+          <t>NF Nº 00000002</t>
         </is>
       </c>
       <c r="D83" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E83" t="n">
-        <v>19210.6</v>
+        <v>227.05</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>CC-0250 - HOSPITAL SÃO LUIZ CAMPINAS</t>
+          <t>CC-0251 - EDIFICIO VIVA!</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>VOTORANTIM CIMENTOS S.A.</t>
+          <t>TELEFONICA BRASIL S.A.</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>NF Nº 00457014-6</t>
+          <t>NF Nº 435274412</t>
         </is>
       </c>
       <c r="D84" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E84" t="n">
-        <v>15730.6</v>
+        <v>1891.31</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>CC-0250 - HOSPITAL SÃO LUIZ CAMPINAS</t>
+          <t>CC-0251 - EDIFICIO VIVA!</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>VOTORANTIM CIMENTOS S.A.</t>
+          <t>TELEFONICA BRASIL S.A.</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>NF Nº 00457214-6</t>
+          <t>NF Nº 455390834</t>
         </is>
       </c>
       <c r="D85" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E85" t="n">
-        <v>6207.6</v>
+        <v>30.67</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>CC-0250 - HOSPITAL SÃO LUIZ CAMPINAS</t>
+          <t>CC-0252 - GRU063 A100 ROW PAULÍNIA - FASE02</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>VOTORANTIM CIMENTOS S.A.</t>
+          <t>ABD COMERCIO DE FERRO E ACO LTDA</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>NF Nº 00457221-6</t>
+          <t>NF Nº 00035672-1</t>
         </is>
       </c>
       <c r="D86" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E86" t="n">
-        <v>6207.6</v>
+        <v>2600</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>CC-0250 - HOSPITAL SÃO LUIZ CAMPINAS</t>
+          <t>CC-0252 - GRU063 A100 ROW PAULÍNIA - FASE02</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>VOTORANTIM CIMENTOS S.A.</t>
+          <t>ADDOR E ASSOCIADOS PROJETOS E CONSULTORIA S/S LTDA</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>NF Nº 00457242-6</t>
+          <t>NF Nº 00003792</t>
         </is>
       </c>
       <c r="D87" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E87" t="n">
-        <v>9321.200000000001</v>
+        <v>8071.1</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>CC-0251 - EDIFICIO VIVA!</t>
+          <t>CC-0252 - GRU063 A100 ROW PAULÍNIA - FASE02</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>CAIXA ECONOMICA FEDERAL</t>
+          <t>AGUAS NASCENTE COMERCIO E PRESTAÇÃO DE SERVIÇO EIRELLI</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>NF Nº 27102022</t>
+          <t>NF Nº 00002580-1</t>
         </is>
       </c>
       <c r="D88" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E88" t="n">
-        <v>5634.35</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>CC-0251 - EDIFICIO VIVA!</t>
+          <t>CC-0252 - GRU063 A100 ROW PAULÍNIA - FASE02</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>EVERTON MACHADO 32468201809</t>
+          <t>CARLOS PRESTES VAZ FIGUEIRA TRANSPORTES - ME</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>NF Nº 00000132</t>
+          <t>NF Nº 00027526</t>
         </is>
       </c>
       <c r="D89" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E89" t="n">
-        <v>1434.78</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>CC-0251 - EDIFICIO VIVA!</t>
+          <t>CC-0252 - GRU063 A100 ROW PAULÍNIA - FASE02</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>SUL AMERICA COMPANHIA DE SEGURO SAUDE</t>
+          <t>Campinas Aluguel de Equipamentos Ltda</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>NF Nº 08423749-0</t>
+          <t>NF Nº 00002766</t>
         </is>
       </c>
       <c r="D90" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E90" t="n">
-        <v>298.62</v>
+        <v>600</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>CC-0251 - EDIFICIO VIVA!</t>
+          <t>CC-0252 - GRU063 A100 ROW PAULÍNIA - FASE02</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>TOKIO MARINE SEGURADORA S.A.</t>
+          <t>LOCAP ANDAIMES LTDA - EPP</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>NF Nº 02591307</t>
+          <t>NF Nº 00002364</t>
         </is>
       </c>
       <c r="D91" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E91" t="n">
-        <v>126.96</v>
+        <v>3200</v>
       </c>
     </row>
     <row r="92">
@@ -2542,19 +2542,19 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>CAIXA ECONOMICA FEDERAL</t>
+          <t>MONTESP COMERCIO E MONTAGENS LTDA</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>NF Nº 271020223</t>
+          <t>NF Nº 00020075</t>
         </is>
       </c>
       <c r="D92" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E92" t="n">
-        <v>6682.75</v>
+        <v>5128.14</v>
       </c>
     </row>
     <row r="93">
@@ -2565,19 +2565,19 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>DRAGOES ESQUADRIAS METALICAS LTDA - ME</t>
+          <t>ORGUEL INDUSTRIA E LOCACAO DE EQUIPAMENTOS S/A</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>NF Nº 00000325</t>
+          <t>NF Nº 00008169</t>
         </is>
       </c>
       <c r="D93" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E93" t="n">
-        <v>111949.81</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="94">
@@ -2588,19 +2588,19 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Fabiano José Vidal</t>
+          <t>SINALL COMERCIO E SERVICOS DE MAQUINAS LTDA</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>NF Nº 00072022</t>
+          <t>NF Nº 00231469</t>
         </is>
       </c>
       <c r="D94" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E94" t="n">
-        <v>2411.99</v>
+        <v>2070.05</v>
       </c>
     </row>
     <row r="95">
@@ -2611,19 +2611,19 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>G.F.C.INDUSTRIA E COMERCIO TUBOS E CONEXOES LTDA</t>
+          <t>STAR CENTER SOLUCOES EM CLIMATIZACAO LTDA</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>NF Nº 00074123-0</t>
+          <t>NF Nº 00000026</t>
         </is>
       </c>
       <c r="D95" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E95" t="n">
-        <v>44999.84</v>
+        <v>188330</v>
       </c>
     </row>
     <row r="96">
@@ -2634,19 +2634,19 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>JOHNSON CONTROLS BE DO BRASIL LTDA.</t>
+          <t>Servicar Paulinia Auto Posto Ltda</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>NF Nº 00039767</t>
+          <t>NF Nº 00004597-2</t>
         </is>
       </c>
       <c r="D96" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E96" t="n">
-        <v>328236.84</v>
+        <v>952.22</v>
       </c>
     </row>
     <row r="97">
@@ -2657,19 +2657,19 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>JOHNSON CONTROLS BE DO BRASIL LTDA.</t>
+          <t>TEMON TECNICA DE MONTAGENS E CONSTRUCOES LTDA</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>NF Nº 00039768</t>
+          <t>NF Nº 00007867</t>
         </is>
       </c>
       <c r="D97" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E97" t="n">
-        <v>314638.95</v>
+        <v>242592.03</v>
       </c>
     </row>
     <row r="98">
@@ -2680,709 +2680,226 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Jairo Norges Cardoso</t>
+          <t>TEMON TECNICA DE MONTAGENS E CONSTRUCOES LTDA</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>NF Nº 00005152</t>
+          <t>NF Nº 00007868</t>
         </is>
       </c>
       <c r="D98" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E98" t="n">
-        <v>13900</v>
+        <v>7263.11</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>CC-0252 - GRU063 A100 ROW PAULÍNIA - FASE02</t>
+          <t>CC-0253 - CITYGATE EXTREMA II</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>M.V. AMBULANCIAS E REMOCOES LTDA</t>
+          <t>CONDOMINIO PORTAL JARDINS D´VERA</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>NF Nº 00000631</t>
+          <t>NF Nº 249428219</t>
         </is>
       </c>
       <c r="D99" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E99" t="n">
-        <v>1200</v>
+        <v>296.99</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>CC-0252 - GRU063 A100 ROW PAULÍNIA - FASE02</t>
+          <t>CC-0253 - CITYGATE EXTREMA II</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Nelson Baldin</t>
+          <t>CONDOMINIO PORTAL JARDINS D´VERA</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>NF Nº 00072022</t>
+          <t>NF Nº 249428528</t>
         </is>
       </c>
       <c r="D100" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E100" t="n">
-        <v>2054.68</v>
+        <v>302.07</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>CC-0252 - GRU063 A100 ROW PAULÍNIA - FASE02</t>
+          <t>CC-0253 - CITYGATE EXTREMA II</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>REIMOLD INDUSTRIA E COMERCIO DE MATERIAIS PLASTICOS LTDA</t>
+          <t>CONDOMINIO PORTAL JARDINS D´VERA</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>NF Nº 00119158-1</t>
+          <t>NF Nº 249428565</t>
         </is>
       </c>
       <c r="D101" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E101" t="n">
-        <v>26136.17</v>
+        <v>302.8</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>CC-0252 - GRU063 A100 ROW PAULÍNIA - FASE02</t>
+          <t>CC-0253 - CITYGATE EXTREMA II</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>RW SOLUÇÃO AMBIENTAL LTDA</t>
+          <t>CONDOMINIO PORTAL JARDINS D´VERA</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>NF Nº 00004396</t>
+          <t>NF Nº 249428583</t>
         </is>
       </c>
       <c r="D102" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E102" t="n">
-        <v>4550</v>
+        <v>302.76</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>CC-0252 - GRU063 A100 ROW PAULÍNIA - FASE02</t>
+          <t>CC-0253 - CITYGATE EXTREMA II</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>SINDICATO DOS TRABALHADORES NAS INDUSTRIAS DA CONST CIVIL E DO MOBILIARIO DE CAMPINAS</t>
+          <t>CONDOMINIO PORTAL JARDINS D´VERA</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>NF Nº 281020222</t>
+          <t>NF Nº 249428735</t>
         </is>
       </c>
       <c r="D103" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E103" t="n">
-        <v>62.42</v>
+        <v>318.54</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>CC-0252 - GRU063 A100 ROW PAULÍNIA - FASE02</t>
+          <t>CC-0253 - CITYGATE EXTREMA II</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>SIPEC COMERCIO REPRESENTACAO IMPORTACAO E SERVICOS LTDA</t>
+          <t>LETICIA WOHLERS DE FREITAS</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>NF Nº 00033307-1</t>
+          <t>NF Nº 00052022</t>
         </is>
       </c>
       <c r="D104" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E104" t="n">
-        <v>5580.66</v>
+        <v>1500.9</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>CC-0252 - GRU063 A100 ROW PAULÍNIA - FASE02</t>
+          <t>CC-0253 - CITYGATE EXTREMA II</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>SQUARE TRAVEL AGENCIA DE VIAGENS E TURISMO - EIRELI</t>
+          <t>MANOEL FERREIRA DE LIMA</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>NF Nº 00004167</t>
+          <t>NF Nº 00072022</t>
         </is>
       </c>
       <c r="D105" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E105" t="n">
-        <v>7365.9</v>
+        <v>360.76</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>CC-0252 - GRU063 A100 ROW PAULÍNIA - FASE02</t>
+          <t>PJ-0246 - PASSEIO PAULISTA PJ</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>SUL AMERICA COMPANHIA DE SEGURO SAUDE</t>
+          <t>PREFEITURA DE SÃO PAULO &lt;IGOR PAULUS MESSIAS MATENAUER TOLEDO - ME&gt;</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>NF Nº 08423749-0</t>
+          <t>NF Nº 00000153-1</t>
         </is>
       </c>
       <c r="D106" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E106" t="n">
-        <v>408.88</v>
+        <v>427.45</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>CC-0252 - GRU063 A100 ROW PAULÍNIA - FASE02</t>
+          <t>PJ-0250 - HOSPITAL SÃO LUIZ CAMPINAS PJ</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>TEMON TECNICA DE MONTAGENS E CONSTRUCOES LTDA</t>
+          <t>PREFEITURA DE SÃO PAULO &lt;SCHALCH CONSTRUÇÕES LTDA&gt;</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>NF Nº 00007795</t>
+          <t>NF Nº 00000035-1</t>
         </is>
       </c>
       <c r="D107" s="2" t="n">
-        <v>44872</v>
+        <v>44935</v>
       </c>
       <c r="E107" t="n">
-        <v>604252.5</v>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="inlineStr">
-        <is>
-          <t>CC-0252 - GRU063 A100 ROW PAULÍNIA - FASE02</t>
-        </is>
-      </c>
-      <c r="B108" t="inlineStr">
-        <is>
-          <t>TOKIO MARINE SEGURADORA S.A.</t>
-        </is>
-      </c>
-      <c r="C108" t="inlineStr">
-        <is>
-          <t>NF Nº 02591307</t>
-        </is>
-      </c>
-      <c r="D108" s="2" t="n">
-        <v>44872</v>
-      </c>
-      <c r="E108" t="n">
-        <v>126.96</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="inlineStr">
-        <is>
-          <t>CC-0252 - GRU063 A100 ROW PAULÍNIA - FASE02</t>
-        </is>
-      </c>
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>TOZZINI,FREIRE,TEIXEIRA,E SILVA ADVOGADOS</t>
-        </is>
-      </c>
-      <c r="C109" t="inlineStr">
-        <is>
-          <t>NF Nº 00097719</t>
-        </is>
-      </c>
-      <c r="D109" s="2" t="n">
-        <v>44872</v>
-      </c>
-      <c r="E109" t="n">
-        <v>7239.11</v>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="inlineStr">
-        <is>
-          <t>CC-0252 - GRU063 A100 ROW PAULÍNIA - FASE02</t>
-        </is>
-      </c>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>Thomas Silva</t>
-        </is>
-      </c>
-      <c r="C110" t="inlineStr">
-        <is>
-          <t>NF Nº 281020222</t>
-        </is>
-      </c>
-      <c r="D110" s="2" t="n">
-        <v>44872</v>
-      </c>
-      <c r="E110" t="n">
-        <v>132.25</v>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="inlineStr">
-        <is>
-          <t>CC-0253 - CITYGATE EXTREMA II</t>
-        </is>
-      </c>
-      <c r="B111" t="inlineStr">
-        <is>
-          <t>CAIXA ECONOMICA FEDERAL</t>
-        </is>
-      </c>
-      <c r="C111" t="inlineStr">
-        <is>
-          <t>NF Nº 27102022</t>
-        </is>
-      </c>
-      <c r="D111" s="2" t="n">
-        <v>44872</v>
-      </c>
-      <c r="E111" t="n">
-        <v>4650.77</v>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="inlineStr">
-        <is>
-          <t>CC-0253 - CITYGATE EXTREMA II</t>
-        </is>
-      </c>
-      <c r="B112" t="inlineStr">
-        <is>
-          <t>LETICIA WOHLERS DE FREITAS</t>
-        </is>
-      </c>
-      <c r="C112" t="inlineStr">
-        <is>
-          <t>NF Nº 00032022</t>
-        </is>
-      </c>
-      <c r="D112" s="2" t="n">
-        <v>44872</v>
-      </c>
-      <c r="E112" t="n">
-        <v>1097.47</v>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="inlineStr">
-        <is>
-          <t>CC-0253 - CITYGATE EXTREMA II</t>
-        </is>
-      </c>
-      <c r="B113" t="inlineStr">
-        <is>
-          <t>LETICIA WOHLERS DE FREITAS</t>
-        </is>
-      </c>
-      <c r="C113" t="inlineStr">
-        <is>
-          <t>NF Nº 00042022</t>
-        </is>
-      </c>
-      <c r="D113" s="2" t="n">
-        <v>44872</v>
-      </c>
-      <c r="E113" t="n">
-        <v>893.05</v>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="inlineStr">
-        <is>
-          <t>CC-0253 - CITYGATE EXTREMA II</t>
-        </is>
-      </c>
-      <c r="B114" t="inlineStr">
-        <is>
-          <t>SOLO NETWORK BRASIL S.A.</t>
-        </is>
-      </c>
-      <c r="C114" t="inlineStr">
-        <is>
-          <t>NF Nº 00076524</t>
-        </is>
-      </c>
-      <c r="D114" s="2" t="n">
-        <v>44872</v>
-      </c>
-      <c r="E114" t="n">
-        <v>16314.92</v>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" t="inlineStr">
-        <is>
-          <t>CC-0253 - CITYGATE EXTREMA II</t>
-        </is>
-      </c>
-      <c r="B115" t="inlineStr">
-        <is>
-          <t>SUL AMERICA COMPANHIA DE SEGURO SAUDE</t>
-        </is>
-      </c>
-      <c r="C115" t="inlineStr">
-        <is>
-          <t>NF Nº 08423749-0</t>
-        </is>
-      </c>
-      <c r="D115" s="2" t="n">
-        <v>44872</v>
-      </c>
-      <c r="E115" t="n">
-        <v>209.22</v>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" t="inlineStr">
-        <is>
-          <t>CC-0253 - CITYGATE EXTREMA II</t>
-        </is>
-      </c>
-      <c r="B116" t="inlineStr">
-        <is>
-          <t>TOKIO MARINE SEGURADORA S.A.</t>
-        </is>
-      </c>
-      <c r="C116" t="inlineStr">
-        <is>
-          <t>NF Nº 02591307</t>
-        </is>
-      </c>
-      <c r="D116" s="2" t="n">
-        <v>44872</v>
-      </c>
-      <c r="E116" t="n">
-        <v>126.93</v>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" t="inlineStr">
-        <is>
-          <t>CC-0254 - DISTRITO ANHEMBI</t>
-        </is>
-      </c>
-      <c r="B117" t="inlineStr">
-        <is>
-          <t>SUL AMERICA COMPANHIA DE SEGURO SAUDE</t>
-        </is>
-      </c>
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>NF Nº 08423749-0</t>
-        </is>
-      </c>
-      <c r="D117" s="2" t="n">
-        <v>44872</v>
-      </c>
-      <c r="E117" t="n">
-        <v>571.9299999999999</v>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" t="inlineStr">
-        <is>
-          <t>JR-0001  - PROCESSOS TRABALHISTAS</t>
-        </is>
-      </c>
-      <c r="B118" t="inlineStr">
-        <is>
-          <t>KONAI, ANDRADE ADVOGADOS ASSOCIADOS</t>
-        </is>
-      </c>
-      <c r="C118" t="inlineStr">
-        <is>
-          <t>NF Nº 00000873</t>
-        </is>
-      </c>
-      <c r="D118" s="2" t="n">
-        <v>44872</v>
-      </c>
-      <c r="E118" t="n">
-        <v>41.4</v>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" t="inlineStr">
-        <is>
-          <t>JR-0002 - PROCESSOS CÍVEIS</t>
-        </is>
-      </c>
-      <c r="B119" t="inlineStr">
-        <is>
-          <t>NACIONAL DE CAMPO GRANDE COMERCIO E SERVICOS DE CONSERVACAO E LIMPEZA LTDA - ME</t>
-        </is>
-      </c>
-      <c r="C119" t="inlineStr">
-        <is>
-          <t>NF Nº 04047088</t>
-        </is>
-      </c>
-      <c r="D119" s="2" t="n">
-        <v>44872</v>
-      </c>
-      <c r="E119" t="n">
-        <v>1510.39</v>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" t="inlineStr">
-        <is>
-          <t>MT-0217  - PARKSHOPPING CAMPO GRANDE MANUTENÇÃO</t>
-        </is>
-      </c>
-      <c r="B120" t="inlineStr">
-        <is>
-          <t>MUNICIPIO DE RIO DE JANEIRO &lt;A J MEGA ESTRUTURA LTDA&gt;</t>
-        </is>
-      </c>
-      <c r="C120" t="inlineStr">
-        <is>
-          <t>NF Nº 00000164</t>
-        </is>
-      </c>
-      <c r="D120" s="2" t="n">
-        <v>44872</v>
-      </c>
-      <c r="E120" t="n">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" t="inlineStr">
-        <is>
-          <t>MT-0217  - PARKSHOPPING CAMPO GRANDE MANUTENÇÃO</t>
-        </is>
-      </c>
-      <c r="B121" t="inlineStr">
-        <is>
-          <t>MUNICIPIO DE RIO DE JANEIRO &lt;A J MEGA ESTRUTURA LTDA&gt;</t>
-        </is>
-      </c>
-      <c r="C121" t="inlineStr">
-        <is>
-          <t>NF Nº 00000179</t>
-        </is>
-      </c>
-      <c r="D121" s="2" t="n">
-        <v>44872</v>
-      </c>
-      <c r="E121" t="n">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" t="inlineStr">
-        <is>
-          <t>MT-0217  - PARKSHOPPING CAMPO GRANDE MANUTENÇÃO</t>
-        </is>
-      </c>
-      <c r="B122" t="inlineStr">
-        <is>
-          <t>MUNICIPIO DE RIO DE JANEIRO &lt;A J MEGA ESTRUTURA LTDA&gt;</t>
-        </is>
-      </c>
-      <c r="C122" t="inlineStr">
-        <is>
-          <t>NF Nº 00000185</t>
-        </is>
-      </c>
-      <c r="D122" s="2" t="n">
-        <v>44872</v>
-      </c>
-      <c r="E122" t="n">
-        <v>1092</v>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" t="inlineStr">
-        <is>
-          <t>MT-CIG   - EQUIPE CIGestçao MANUTENÇÃO</t>
-        </is>
-      </c>
-      <c r="B123" t="inlineStr">
-        <is>
-          <t>CAIXA ECONOMICA FEDERAL</t>
-        </is>
-      </c>
-      <c r="C123" t="inlineStr">
-        <is>
-          <t>NF Nº 27102022</t>
-        </is>
-      </c>
-      <c r="D123" s="2" t="n">
-        <v>44872</v>
-      </c>
-      <c r="E123" t="n">
-        <v>1094.77</v>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" t="inlineStr">
-        <is>
-          <t>MT-CIG   - EQUIPE CIGestçao MANUTENÇÃO</t>
-        </is>
-      </c>
-      <c r="B124" t="inlineStr">
-        <is>
-          <t>FABIO FRANCISCO OLIVEIRA DA SILVA</t>
-        </is>
-      </c>
-      <c r="C124" t="inlineStr">
-        <is>
-          <t>NF Nº 07112022</t>
-        </is>
-      </c>
-      <c r="D124" s="2" t="n">
-        <v>44872</v>
-      </c>
-      <c r="E124" t="n">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" t="inlineStr">
-        <is>
-          <t>MT-CIG   - EQUIPE CIGestçao MANUTENÇÃO</t>
-        </is>
-      </c>
-      <c r="B125" t="inlineStr">
-        <is>
-          <t>SUL AMERICA COMPANHIA DE SEGURO SAUDE</t>
-        </is>
-      </c>
-      <c r="C125" t="inlineStr">
-        <is>
-          <t>NF Nº 08423749-0</t>
-        </is>
-      </c>
-      <c r="D125" s="2" t="n">
-        <v>44872</v>
-      </c>
-      <c r="E125" t="n">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" t="inlineStr">
-        <is>
-          <t>RT-0001  - RESCISÕES</t>
-        </is>
-      </c>
-      <c r="B126" t="inlineStr">
-        <is>
-          <t>CAIXA ECONOMICA FEDERAL</t>
-        </is>
-      </c>
-      <c r="C126" t="inlineStr">
-        <is>
-          <t>NF Nº 31102022</t>
-        </is>
-      </c>
-      <c r="D126" s="2" t="n">
-        <v>44872</v>
-      </c>
-      <c r="E126" t="n">
-        <v>31094.21</v>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" t="inlineStr">
-        <is>
-          <t>RT-0001  - RESCISÕES</t>
-        </is>
-      </c>
-      <c r="B127" t="inlineStr">
-        <is>
-          <t>CONSTRUTORA FONSECA &amp; MERCADANTE LTDA</t>
-        </is>
-      </c>
-      <c r="C127" t="inlineStr">
-        <is>
-          <t>NF Nº 31102022</t>
-        </is>
-      </c>
-      <c r="D127" s="2" t="n">
-        <v>44872</v>
-      </c>
-      <c r="E127" t="n">
-        <v>46331.03</v>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" t="inlineStr">
-        <is>
-          <t>RT-0001  - RESCISÕES</t>
-        </is>
-      </c>
-      <c r="B128" t="inlineStr">
-        <is>
-          <t>LILIAN MARTINS BARREIRA - ME</t>
-        </is>
-      </c>
-      <c r="C128" t="inlineStr">
-        <is>
-          <t>NF Nº 01112022</t>
-        </is>
-      </c>
-      <c r="D128" s="2" t="n">
-        <v>44872</v>
-      </c>
-      <c r="E128" t="n">
-        <v>68707.95</v>
+        <v>736.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>